<commit_message>
Article and figure fixes: legend, table fit, maps, machine-readable text, uniform-set symmetry
- Sectoral figure: legend shows Maule/Canterbury instead of Chile/NZ
- Sectoral table: resize to text width for page fit
- Maps: increase height from 0.2 to 0.3 textheight (+50%)
- Remove file-path sentences; use replication-package notes
- Uniform-set sensitivity: NZ uses pre-fit threshold (2x, 5x, 10x) like Chile; drop treatment-year panels (covered by timing and in-time placebo)

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/article_assets/sectoral_appendix_series.xlsx
+++ b/article_assets/sectoral_appendix_series.xlsx
@@ -119,16 +119,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -144,7 +136,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -152,30 +144,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,25 +451,25 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -516,10 +490,10 @@
         <v>0.04691903419910123</v>
       </c>
       <c r="F2">
-        <v>0.04903914328371776</v>
+        <v>0.04914754552340982</v>
       </c>
       <c r="G2">
-        <v>-0.002120109084616538</v>
+        <v>-0.002228511324308589</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -539,10 +513,10 @@
         <v>0.04668696534725243</v>
       </c>
       <c r="F3">
-        <v>0.04653368389526427</v>
+        <v>0.04642298833034395</v>
       </c>
       <c r="G3">
-        <v>0.0001532814519881534</v>
+        <v>0.0002639770169084801</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -562,10 +536,10 @@
         <v>0.04817567567567568</v>
       </c>
       <c r="F4">
-        <v>0.04756270102225354</v>
+        <v>0.04746439240901662</v>
       </c>
       <c r="G4">
-        <v>0.0006129746534221381</v>
+        <v>0.000711283266659056</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -585,10 +559,10 @@
         <v>0.05033557046979865</v>
       </c>
       <c r="F5">
-        <v>0.05108711806470673</v>
+        <v>0.05101704205014047</v>
       </c>
       <c r="G5">
-        <v>-0.0007515475949080724</v>
+        <v>-0.0006814715803418192</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -608,10 +582,10 @@
         <v>0.05379746835443038</v>
       </c>
       <c r="F6">
-        <v>0.05337222349760743</v>
+        <v>0.05332612913267411</v>
       </c>
       <c r="G6">
-        <v>0.0004252448568229511</v>
+        <v>0.0004713392217562742</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -631,10 +605,10 @@
         <v>0.06148572652777034</v>
       </c>
       <c r="F7">
-        <v>0.06183898621969081</v>
+        <v>0.06175142344466621</v>
       </c>
       <c r="G7">
-        <v>-0.0003532596919204739</v>
+        <v>-0.0002656969168958676</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -654,10 +628,10 @@
         <v>0.05970452353150226</v>
       </c>
       <c r="F8">
-        <v>0.05782189214230722</v>
+        <v>0.05794548726702072</v>
       </c>
       <c r="G8">
-        <v>0.00188263138919504</v>
+        <v>0.001759036264481539</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -677,10 +651,10 @@
         <v>0.06115056479672084</v>
       </c>
       <c r="F9">
-        <v>0.06130501919439296</v>
+        <v>0.0612030479019746</v>
       </c>
       <c r="G9">
-        <v>-0.0001544543976721158</v>
+        <v>-5.248310525376304E-05</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -700,10 +674,10 @@
         <v>0.06523373579231348</v>
       </c>
       <c r="F10">
-        <v>0.06412075855941621</v>
+        <v>0.06425910732455484</v>
       </c>
       <c r="G10">
-        <v>0.001112977232897272</v>
+        <v>0.0009746284677586425</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -723,10 +697,10 @@
         <v>0.0607488647073944</v>
       </c>
       <c r="F11">
-        <v>0.06180542847574513</v>
+        <v>0.06176683645603889</v>
       </c>
       <c r="G11">
-        <v>-0.001056563768350727</v>
+        <v>-0.001017971748644486</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -746,10 +720,10 @@
         <v>0.05813177648040033</v>
       </c>
       <c r="F12">
-        <v>0.06159272356671482</v>
+        <v>0.06147517124408719</v>
       </c>
       <c r="G12">
-        <v>-0.003460947086314482</v>
+        <v>-0.003343394763686856</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -769,10 +743,10 @@
         <v>0.05822814955941891</v>
       </c>
       <c r="F13">
-        <v>0.05783171154824718</v>
+        <v>0.05764441586953398</v>
       </c>
       <c r="G13">
-        <v>0.0003964380111717222</v>
+        <v>0.0005837336898849299</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -792,10 +766,10 @@
         <v>0.06914873572747485</v>
       </c>
       <c r="F14">
-        <v>0.05403581429908177</v>
+        <v>0.05372037583401951</v>
       </c>
       <c r="G14">
-        <v>0.01511292142839307</v>
+        <v>0.01542835989345533</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -815,10 +789,10 @@
         <v>0.08298755186721991</v>
       </c>
       <c r="F15">
-        <v>0.05675334739655347</v>
+        <v>0.05654634625019033</v>
       </c>
       <c r="G15">
-        <v>0.02623420447066644</v>
+        <v>0.02644120561702958</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -838,10 +812,10 @@
         <v>0.08872620790629575</v>
       </c>
       <c r="F16">
-        <v>0.05518360399993378</v>
+        <v>0.05508391155110233</v>
       </c>
       <c r="G16">
-        <v>0.03354260390636197</v>
+        <v>0.03364229635519342</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -861,10 +835,10 @@
         <v>0.0983616769451193</v>
       </c>
       <c r="F17">
-        <v>0.05753326288390682</v>
+        <v>0.05749427974624747</v>
       </c>
       <c r="G17">
-        <v>0.04082841406121248</v>
+        <v>0.04086739719887183</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -884,10 +858,10 @@
         <v>0.09969214052879391</v>
       </c>
       <c r="F18">
-        <v>0.05947103106305311</v>
+        <v>0.0595106712358233</v>
       </c>
       <c r="G18">
-        <v>0.0402211094657408</v>
+        <v>0.04018146929297061</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -907,10 +881,10 @@
         <v>0.09143342311746105</v>
       </c>
       <c r="F19">
-        <v>0.06223947017237548</v>
+        <v>0.0624501643347157</v>
       </c>
       <c r="G19">
-        <v>0.02919395294508557</v>
+        <v>0.02898325878274536</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -930,10 +904,10 @@
         <v>0.08983619068385619</v>
       </c>
       <c r="F20">
-        <v>0.06587000586410884</v>
+        <v>0.06606117393067792</v>
       </c>
       <c r="G20">
-        <v>0.02396618481974735</v>
+        <v>0.02377501675317827</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -953,10 +927,10 @@
         <v>0.08674308692586886</v>
       </c>
       <c r="F21">
-        <v>0.06845449964216656</v>
+        <v>0.06869522871930629</v>
       </c>
       <c r="G21">
-        <v>0.01828858728370231</v>
+        <v>0.01804785820656257</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -976,10 +950,10 @@
         <v>0.9530809658008987</v>
       </c>
       <c r="F22">
-        <v>0.9542286473815622</v>
+        <v>0.9542276710690105</v>
       </c>
       <c r="G22">
-        <v>-0.001147681580663473</v>
+        <v>-0.001146705268111781</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -999,10 +973,10 @@
         <v>0.9533130346527475</v>
       </c>
       <c r="F23">
-        <v>0.954881204074449</v>
+        <v>0.9548837430518627</v>
       </c>
       <c r="G23">
-        <v>-0.00156816942170146</v>
+        <v>-0.001570708399115217</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1022,10 +996,10 @@
         <v>0.9518243243243243</v>
       </c>
       <c r="F24">
-        <v>0.9539820221272626</v>
+        <v>0.9539830934528754</v>
       </c>
       <c r="G24">
-        <v>-0.002157697802938285</v>
+        <v>-0.002158769128551064</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1045,10 +1019,10 @@
         <v>0.9496644295302014</v>
       </c>
       <c r="F25">
-        <v>0.9486791506758953</v>
+        <v>0.9486783806997667</v>
       </c>
       <c r="G25">
-        <v>0.0009852788543061042</v>
+        <v>0.0009860488304346271</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1068,10 +1042,10 @@
         <v>0.9462025316455697</v>
       </c>
       <c r="F26">
-        <v>0.9463988667579621</v>
+        <v>0.9463989042561163</v>
       </c>
       <c r="G26">
-        <v>-0.0001963351123924761</v>
+        <v>-0.0001963726105466135</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1091,10 +1065,10 @@
         <v>0.9385142734722297</v>
       </c>
       <c r="F27">
-        <v>0.9402248620654423</v>
+        <v>0.9402243425339858</v>
       </c>
       <c r="G27">
-        <v>-0.001710588593212603</v>
+        <v>-0.001710069061756081</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1114,10 +1088,10 @@
         <v>0.9402954764684978</v>
       </c>
       <c r="F28">
-        <v>0.9411956256421238</v>
+        <v>0.9411943646902954</v>
       </c>
       <c r="G28">
-        <v>-0.0009001491736260192</v>
+        <v>-0.0008988882217976224</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1137,10 +1111,10 @@
         <v>0.9388494352032791</v>
       </c>
       <c r="F29">
-        <v>0.9356067557327887</v>
+        <v>0.9356069417465607</v>
       </c>
       <c r="G29">
-        <v>0.003242679470490395</v>
+        <v>0.003242493456718454</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1160,10 +1134,10 @@
         <v>0.9347662642076865</v>
       </c>
       <c r="F30">
-        <v>0.9351163840592994</v>
+        <v>0.9351166782000135</v>
       </c>
       <c r="G30">
-        <v>-0.0003501198516129289</v>
+        <v>-0.0003504139923270477</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1183,10 +1157,10 @@
         <v>0.9392511352926056</v>
       </c>
       <c r="F31">
-        <v>0.9368485104525452</v>
+        <v>0.9368499297440585</v>
       </c>
       <c r="G31">
-        <v>0.002402624840060374</v>
+        <v>0.002401205548547169</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1206,10 +1180,10 @@
         <v>0.9418682235195996</v>
       </c>
       <c r="F32">
-        <v>0.9329022138310994</v>
+        <v>0.9329059477386188</v>
       </c>
       <c r="G32">
-        <v>0.008966009688500254</v>
+        <v>0.008962275780980855</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1229,10 +1203,10 @@
         <v>0.9417718504405811</v>
       </c>
       <c r="F33">
-        <v>0.9363559258112988</v>
+        <v>0.9363603637113479</v>
       </c>
       <c r="G33">
-        <v>0.005415924629282309</v>
+        <v>0.005411486729233195</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1252,10 +1226,10 @@
         <v>0.9308512642725252</v>
       </c>
       <c r="F34">
-        <v>0.9383681418927015</v>
+        <v>0.9383738226470104</v>
       </c>
       <c r="G34">
-        <v>-0.007516877620176277</v>
+        <v>-0.007522558374485233</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1275,10 +1249,10 @@
         <v>0.91701244813278</v>
       </c>
       <c r="F35">
-        <v>0.9376094562032649</v>
+        <v>0.9376153013878925</v>
       </c>
       <c r="G35">
-        <v>-0.02059700807048481</v>
+        <v>-0.02060285325511246</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1298,10 +1272,10 @@
         <v>0.9112737920937043</v>
       </c>
       <c r="F36">
-        <v>0.9417102061346343</v>
+        <v>0.9417166644204169</v>
       </c>
       <c r="G36">
-        <v>-0.03043641404093</v>
+        <v>-0.03044287232671261</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1321,10 +1295,10 @@
         <v>0.9016383230548807</v>
       </c>
       <c r="F37">
-        <v>0.9367642336422186</v>
+        <v>0.9367718883734395</v>
       </c>
       <c r="G37">
-        <v>-0.03512591058733794</v>
+        <v>-0.03513356531855882</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1344,10 +1318,10 @@
         <v>0.9003078594712061</v>
       </c>
       <c r="F38">
-        <v>0.9336398404284197</v>
+        <v>0.933647591730317</v>
       </c>
       <c r="G38">
-        <v>-0.03333198095721368</v>
+        <v>-0.03333973225911091</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1367,10 +1341,10 @@
         <v>0.9085665768825389</v>
       </c>
       <c r="F39">
-        <v>0.935514893725911</v>
+        <v>0.9355212226455755</v>
       </c>
       <c r="G39">
-        <v>-0.02694831684337207</v>
+        <v>-0.02695464576303652</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1390,10 +1364,10 @@
         <v>0.9101638093161438</v>
       </c>
       <c r="F40">
-        <v>0.9329064478761071</v>
+        <v>0.9329126582449331</v>
       </c>
       <c r="G40">
-        <v>-0.02274263855996328</v>
+        <v>-0.02274884892878926</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1413,10 +1387,10 @@
         <v>0.9132569130741311</v>
       </c>
       <c r="F41">
-        <v>0.9340366748841253</v>
+        <v>0.9340425647508108</v>
       </c>
       <c r="G41">
-        <v>-0.02077976180999419</v>
+        <v>-0.02078565167667967</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1436,10 +1410,10 @@
         <v>12513</v>
       </c>
       <c r="F42">
-        <v>12843.63426589029</v>
+        <v>12856.71379678796</v>
       </c>
       <c r="G42">
-        <v>-330.6342658902922</v>
+        <v>-343.7137967879644</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1459,10 +1433,10 @@
         <v>13150</v>
       </c>
       <c r="F43">
-        <v>13326.09696772344</v>
+        <v>13436.06298007441</v>
       </c>
       <c r="G43">
-        <v>-176.0969677234443</v>
+        <v>-286.0629800744136</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1482,10 +1456,10 @@
         <v>14087</v>
       </c>
       <c r="F44">
-        <v>14369.98966864331</v>
+        <v>14490.22338908094</v>
       </c>
       <c r="G44">
-        <v>-282.9896686433112</v>
+        <v>-403.2233890809366</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1505,10 +1479,10 @@
         <v>14999</v>
       </c>
       <c r="F45">
-        <v>15522.17361445871</v>
+        <v>15449.11667928596</v>
       </c>
       <c r="G45">
-        <v>-523.1736144587085</v>
+        <v>-450.116679285964</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1528,10 +1502,10 @@
         <v>16146</v>
       </c>
       <c r="F46">
-        <v>16658.76020726084</v>
+        <v>16549.98429227336</v>
       </c>
       <c r="G46">
-        <v>-512.7602072608424</v>
+        <v>-403.9842922733624</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1551,10 +1525,10 @@
         <v>17523</v>
       </c>
       <c r="F47">
-        <v>17866.14490439508</v>
+        <v>17715.53218517026</v>
       </c>
       <c r="G47">
-        <v>-343.1449043950779</v>
+        <v>-192.5321851702574</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1574,10 +1548,10 @@
         <v>18521</v>
       </c>
       <c r="F48">
-        <v>18705.28914014521</v>
+        <v>18624.21069046617</v>
       </c>
       <c r="G48">
-        <v>-184.2891401452107</v>
+        <v>-103.2106904661705</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1597,10 +1571,10 @@
         <v>19698</v>
       </c>
       <c r="F49">
-        <v>19392.06617005379</v>
+        <v>19409.45023664171</v>
       </c>
       <c r="G49">
-        <v>305.933829946207</v>
+        <v>288.5497633582927</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1620,10 +1594,10 @@
         <v>21136</v>
       </c>
       <c r="F50">
-        <v>20830.05021751628</v>
+        <v>20814.31547533565</v>
       </c>
       <c r="G50">
-        <v>305.9497824837235</v>
+        <v>321.6845246643497</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1643,10 +1617,10 @@
         <v>21924</v>
       </c>
       <c r="F51">
-        <v>20762.98318225572</v>
+        <v>20888.1071342718</v>
       </c>
       <c r="G51">
-        <v>1161.016817744276</v>
+        <v>1035.892865728201</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1666,10 +1640,10 @@
         <v>22586</v>
       </c>
       <c r="F52">
-        <v>21514.07131792587</v>
+        <v>21550.80365371035</v>
       </c>
       <c r="G52">
-        <v>1071.928682074125</v>
+        <v>1035.196346289649</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1689,10 +1663,10 @@
         <v>23727</v>
       </c>
       <c r="F53">
-        <v>22515.38445240293</v>
+        <v>22566.07458544222</v>
       </c>
       <c r="G53">
-        <v>1211.615547597074</v>
+        <v>1160.92541455778</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1712,10 +1686,10 @@
         <v>24702</v>
       </c>
       <c r="F54">
-        <v>23729.99814013089</v>
+        <v>23802.97895723172</v>
       </c>
       <c r="G54">
-        <v>972.0018598691095</v>
+        <v>899.0210427682759</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1735,10 +1709,10 @@
         <v>25415</v>
       </c>
       <c r="F55">
-        <v>24429.35588075684</v>
+        <v>24372.31008384826</v>
       </c>
       <c r="G55">
-        <v>985.6441192431557</v>
+        <v>1042.689916151743</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1758,10 +1732,10 @@
         <v>28008</v>
       </c>
       <c r="F56">
-        <v>25788.69835868197</v>
+        <v>25821.29942783882</v>
       </c>
       <c r="G56">
-        <v>2219.301641318034</v>
+        <v>2186.700572161182</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1781,10 +1755,10 @@
         <v>28948</v>
       </c>
       <c r="F57">
-        <v>27407.32402474498</v>
+        <v>27251.64125749184</v>
       </c>
       <c r="G57">
-        <v>1540.675975255017</v>
+        <v>1696.358742508164</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1804,10 +1778,10 @@
         <v>29829</v>
       </c>
       <c r="F58">
-        <v>29551.81975796131</v>
+        <v>29252.36126056217</v>
       </c>
       <c r="G58">
-        <v>277.1802420386921</v>
+        <v>576.6387394378289</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1827,10 +1801,10 @@
         <v>31033</v>
       </c>
       <c r="F59">
-        <v>31339.93291469495</v>
+        <v>31070.5995027171</v>
       </c>
       <c r="G59">
-        <v>-306.9329146949494</v>
+        <v>-37.59950271710477</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1850,10 +1824,10 @@
         <v>33393</v>
       </c>
       <c r="F60">
-        <v>33211.53144962769</v>
+        <v>32972.4054598879</v>
       </c>
       <c r="G60">
-        <v>181.4685503723085</v>
+        <v>420.5945401120989</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1873,10 +1847,10 @@
         <v>34975</v>
       </c>
       <c r="F61">
-        <v>34954.85012121683</v>
+        <v>34719.29188398688</v>
       </c>
       <c r="G61">
-        <v>20.14987878317334</v>
+        <v>255.7081160131202</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1896,10 +1870,10 @@
         <v>0.1252065879138082</v>
       </c>
       <c r="F62">
-        <v>0.1075480861304017</v>
+        <v>0.1075479550173169</v>
       </c>
       <c r="G62">
-        <v>0.01765850178340647</v>
+        <v>0.01765863289649129</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1919,10 +1893,10 @@
         <v>0.1270521143564077</v>
       </c>
       <c r="F63">
-        <v>0.09419979257666328</v>
+        <v>0.09419958929454807</v>
       </c>
       <c r="G63">
-        <v>0.0328523217797444</v>
+        <v>0.03285252506185961</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1942,10 +1916,10 @@
         <v>0.09640065513227573</v>
       </c>
       <c r="F64">
-        <v>0.08723358514931133</v>
+        <v>0.08723342996826171</v>
       </c>
       <c r="G64">
-        <v>0.009167069982964404</v>
+        <v>0.009167225164014026</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1965,10 +1939,10 @@
         <v>0.1039011569877813</v>
       </c>
       <c r="F65">
-        <v>0.09154980720930508</v>
+        <v>0.09154972602756158</v>
       </c>
       <c r="G65">
-        <v>0.01235134977847625</v>
+        <v>0.01235143096021976</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1988,10 +1962,10 @@
         <v>0.09676342620177571</v>
       </c>
       <c r="F66">
-        <v>0.09703580940000743</v>
+        <v>0.09703578461130455</v>
       </c>
       <c r="G66">
-        <v>-0.0002723831982317237</v>
+        <v>-0.0002723584095288417</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2011,10 +1985,10 @@
         <v>0.09758212037682651</v>
       </c>
       <c r="F67">
-        <v>0.09820962904852823</v>
+        <v>0.0982094592899327</v>
       </c>
       <c r="G67">
-        <v>-0.0006275086717017209</v>
+        <v>-0.0006273389131061929</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2034,10 +2008,10 @@
         <v>0.1083456446593851</v>
       </c>
       <c r="F68">
-        <v>0.0995737391388857</v>
+        <v>0.09957373795334637</v>
       </c>
       <c r="G68">
-        <v>0.008771905520499418</v>
+        <v>0.008771906706038751</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2057,10 +2031,10 @@
         <v>0.1006909402678728</v>
       </c>
       <c r="F69">
-        <v>0.09996796762683217</v>
+        <v>0.09996811793050285</v>
       </c>
       <c r="G69">
-        <v>0.000722972641040584</v>
+        <v>0.0007228223373699078</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2080,10 +2054,10 @@
         <v>0.1007299776494794</v>
       </c>
       <c r="F70">
-        <v>0.1023235850377843</v>
+        <v>0.1023237112253731</v>
       </c>
       <c r="G70">
-        <v>-0.001593607388304913</v>
+        <v>-0.001593733575893749</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2103,10 +2077,10 @@
         <v>0.1139124398085379</v>
       </c>
       <c r="F71">
-        <v>0.1061266136776063</v>
+        <v>0.1061267858999395</v>
       </c>
       <c r="G71">
-        <v>0.007785826130931553</v>
+        <v>0.007785653908598367</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2126,10 +2100,10 @@
         <v>0.1057113322015655</v>
       </c>
       <c r="F72">
-        <v>0.1086960811447516</v>
+        <v>0.1086961312584513</v>
       </c>
       <c r="G72">
-        <v>-0.002984748943186094</v>
+        <v>-0.00298479905688584</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -2149,10 +2123,10 @@
         <v>0.09298192490037074</v>
       </c>
       <c r="F73">
-        <v>0.08913111924959125</v>
+        <v>0.08913104645874996</v>
       </c>
       <c r="G73">
-        <v>0.003850805650779499</v>
+        <v>0.003850878441620784</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -2172,10 +2146,10 @@
         <v>0.07856868751026944</v>
       </c>
       <c r="F74">
-        <v>0.09874485027544158</v>
+        <v>0.09874464854641272</v>
       </c>
       <c r="G74">
-        <v>-0.02017616276517215</v>
+        <v>-0.02017596103614329</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2195,10 +2169,10 @@
         <v>0.07372633789242261</v>
       </c>
       <c r="F75">
-        <v>0.09378138890638987</v>
+        <v>0.09378132011033277</v>
       </c>
       <c r="G75">
-        <v>-0.02005505101396726</v>
+        <v>-0.02005498221791016</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2218,10 +2192,10 @@
         <v>0.07444375461985837</v>
       </c>
       <c r="F76">
-        <v>0.08316635735948218</v>
+        <v>0.0831660963105755</v>
       </c>
       <c r="G76">
-        <v>-0.008722602739623803</v>
+        <v>-0.008722341690717131</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -2241,10 +2215,10 @@
         <v>0.08002806486274189</v>
       </c>
       <c r="F77">
-        <v>0.08312732209793401</v>
+        <v>0.08312712698714364</v>
       </c>
       <c r="G77">
-        <v>-0.003099257235192124</v>
+        <v>-0.003099062124401752</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -2264,10 +2238,10 @@
         <v>0.07880202852295674</v>
       </c>
       <c r="F78">
-        <v>0.08493953032930904</v>
+        <v>0.08493933870294451</v>
       </c>
       <c r="G78">
-        <v>-0.006137501806352294</v>
+        <v>-0.006137310179987768</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2287,10 +2261,10 @@
         <v>0.0651327115527794</v>
       </c>
       <c r="F79">
-        <v>0.08631040706393225</v>
+        <v>0.08631036401228892</v>
       </c>
       <c r="G79">
-        <v>-0.02117769551115285</v>
+        <v>-0.02117765245950952</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2310,10 +2284,10 @@
         <v>0.07696465401615833</v>
       </c>
       <c r="F80">
-        <v>0.08071617291343262</v>
+        <v>0.08071615204932318</v>
       </c>
       <c r="G80">
-        <v>-0.003751518897274292</v>
+        <v>-0.003751498033164852</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -2333,10 +2307,10 @@
         <v>0.06750063001115154</v>
       </c>
       <c r="F81">
-        <v>0.08984351353856143</v>
+        <v>0.08984355740497152</v>
       </c>
       <c r="G81">
-        <v>-0.02234288352740989</v>
+        <v>-0.02234292739381998</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -2356,10 +2330,10 @@
         <v>0.08794814508824059</v>
       </c>
       <c r="F82">
-        <v>0.07186920518548565</v>
+        <v>0.0718692295769951</v>
       </c>
       <c r="G82">
-        <v>0.01607893990275494</v>
+        <v>0.01607891551124549</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2379,10 +2353,10 @@
         <v>0.08926860563214774</v>
       </c>
       <c r="F83">
-        <v>0.08211460606892898</v>
+        <v>0.08211461587099765</v>
       </c>
       <c r="G83">
-        <v>0.007153999563218758</v>
+        <v>0.007153989761150087</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2402,10 +2376,10 @@
         <v>0.106741440143696</v>
       </c>
       <c r="F84">
-        <v>0.07083990285401556</v>
+        <v>0.07083981474515837</v>
       </c>
       <c r="G84">
-        <v>0.03590153728968044</v>
+        <v>0.03590162539853764</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -2425,10 +2399,10 @@
         <v>0.09271746053033304</v>
       </c>
       <c r="F85">
-        <v>0.07074509873421059</v>
+        <v>0.07074496775474372</v>
       </c>
       <c r="G85">
-        <v>0.02197236179612246</v>
+        <v>0.02197249277558933</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2448,10 +2422,10 @@
         <v>0.08269758493423586</v>
       </c>
       <c r="F86">
-        <v>0.06687523054348007</v>
+        <v>0.06687515561952979</v>
       </c>
       <c r="G86">
-        <v>0.01582235439075579</v>
+        <v>0.01582242931470607</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -2471,10 +2445,10 @@
         <v>0.08798046295695597</v>
       </c>
       <c r="F87">
-        <v>0.07557351380512496</v>
+        <v>0.07557337962217253</v>
       </c>
       <c r="G87">
-        <v>0.01240694915183101</v>
+        <v>0.01240708333478344</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -2494,10 +2468,10 @@
         <v>0.8747934120861918</v>
       </c>
       <c r="F88">
-        <v>0.8967010409612292</v>
+        <v>0.8967010403087794</v>
       </c>
       <c r="G88">
-        <v>-0.02190762887503739</v>
+        <v>-0.02190762822258763</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2517,10 +2491,10 @@
         <v>0.8729478856435924</v>
       </c>
       <c r="F89">
-        <v>0.9120725522203377</v>
+        <v>0.9120725517911055</v>
       </c>
       <c r="G89">
-        <v>-0.03912466657674529</v>
+        <v>-0.03912466614751309</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2540,10 +2514,10 @@
         <v>0.9035993448677243</v>
       </c>
       <c r="F90">
-        <v>0.9173105529819141</v>
+        <v>0.917310553104472</v>
       </c>
       <c r="G90">
-        <v>-0.0137112081141898</v>
+        <v>-0.01371120823674765</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2563,10 +2537,10 @@
         <v>0.8960988430122186</v>
       </c>
       <c r="F91">
-        <v>0.9107733118950196</v>
+        <v>0.9107733120589669</v>
       </c>
       <c r="G91">
-        <v>-0.014674468882801</v>
+        <v>-0.0146744690467483</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2586,10 +2560,10 @@
         <v>0.9032365737982243</v>
       </c>
       <c r="F92">
-        <v>0.9038989001361122</v>
+        <v>0.9038988997704152</v>
       </c>
       <c r="G92">
-        <v>-0.0006623263378878752</v>
+        <v>-0.000662325972190847</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2609,10 +2583,10 @@
         <v>0.9024178796231734</v>
       </c>
       <c r="F93">
-        <v>0.9068599690575325</v>
+        <v>0.9068599690097128</v>
       </c>
       <c r="G93">
-        <v>-0.004442089434359087</v>
+        <v>-0.004442089386539338</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2632,10 +2606,10 @@
         <v>0.8916543553406149</v>
       </c>
       <c r="F94">
-        <v>0.9002415234611032</v>
+        <v>0.90024152386692</v>
       </c>
       <c r="G94">
-        <v>-0.00858716812048832</v>
+        <v>-0.008587168526305144</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2655,10 +2629,10 @@
         <v>0.8993090597321273</v>
       </c>
       <c r="F95">
-        <v>0.8951321154176819</v>
+        <v>0.8951321162188727</v>
       </c>
       <c r="G95">
-        <v>0.004176944314445374</v>
+        <v>0.004176943513254594</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2678,10 +2652,10 @@
         <v>0.8992700223505207</v>
       </c>
       <c r="F96">
-        <v>0.8942325890211198</v>
+        <v>0.8942325884578204</v>
       </c>
       <c r="G96">
-        <v>0.005037433329400876</v>
+        <v>0.005037433892700283</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2701,10 +2675,10 @@
         <v>0.8860875601914622</v>
       </c>
       <c r="F97">
-        <v>0.8894418652630833</v>
+        <v>0.8894418639986325</v>
       </c>
       <c r="G97">
-        <v>-0.003354305071621155</v>
+        <v>-0.003354303807170278</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2724,10 +2698,10 @@
         <v>0.8942886677984345</v>
       </c>
       <c r="F98">
-        <v>0.8905763462955423</v>
+        <v>0.890576344890889</v>
       </c>
       <c r="G98">
-        <v>0.003712321502892246</v>
+        <v>0.003712322907545529</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2747,10 +2721,10 @@
         <v>0.9070180750996293</v>
       </c>
       <c r="F99">
-        <v>0.913575168161871</v>
+        <v>0.9135751671589434</v>
       </c>
       <c r="G99">
-        <v>-0.006557093062241726</v>
+        <v>-0.006557092059314096</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2770,10 +2744,10 @@
         <v>0.9214313124897305</v>
       </c>
       <c r="F100">
-        <v>0.9078272402920177</v>
+        <v>0.9078272392246365</v>
       </c>
       <c r="G100">
-        <v>0.01360407219771287</v>
+        <v>0.01360407326509405</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2793,10 +2767,10 @@
         <v>0.9262736621075773</v>
       </c>
       <c r="F101">
-        <v>0.9082185374877274</v>
+        <v>0.9082185375690264</v>
       </c>
       <c r="G101">
-        <v>0.01805512461984993</v>
+        <v>0.01805512453855096</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2816,10 +2790,10 @@
         <v>0.9255562453801416</v>
       </c>
       <c r="F102">
-        <v>0.9248824045902887</v>
+        <v>0.9248824040501483</v>
       </c>
       <c r="G102">
-        <v>0.0006738407898528864</v>
+        <v>0.0006738413299932633</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2839,10 +2813,10 @@
         <v>0.9199719351372582</v>
       </c>
       <c r="F103">
-        <v>0.9230562135568963</v>
+        <v>0.9230562128436003</v>
       </c>
       <c r="G103">
-        <v>-0.003084278419638098</v>
+        <v>-0.00308427770634212</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2862,10 +2836,10 @@
         <v>0.9211979714770433</v>
       </c>
       <c r="F104">
-        <v>0.9212689763080356</v>
+        <v>0.9212689753576703</v>
       </c>
       <c r="G104">
-        <v>-7.100483099231614E-05</v>
+        <v>-7.100388062697416E-05</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2885,10 +2859,10 @@
         <v>0.9348672884472206</v>
       </c>
       <c r="F105">
-        <v>0.9154536799549069</v>
+        <v>0.9154536790601345</v>
       </c>
       <c r="G105">
-        <v>0.01941360849231366</v>
+        <v>0.01941360938708603</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2908,10 +2882,10 @@
         <v>0.9230353459838416</v>
       </c>
       <c r="F106">
-        <v>0.9202027430971363</v>
+        <v>0.9202027425454504</v>
       </c>
       <c r="G106">
-        <v>0.002832602886705282</v>
+        <v>0.002832603438391201</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2931,10 +2905,10 @@
         <v>0.9324993699888484</v>
       </c>
       <c r="F107">
-        <v>0.9092438372635219</v>
+        <v>0.909243836542772</v>
       </c>
       <c r="G107">
-        <v>0.02325553272532654</v>
+        <v>0.02325553344607645</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2954,10 +2928,10 @@
         <v>0.9120518549117594</v>
       </c>
       <c r="F108">
-        <v>0.9276477162199837</v>
+        <v>0.9276477157742163</v>
       </c>
       <c r="G108">
-        <v>-0.01559586130822421</v>
+        <v>-0.0155958608624569</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2977,10 +2951,10 @@
         <v>0.9107313943678522</v>
       </c>
       <c r="F109">
-        <v>0.9177318245308423</v>
+        <v>0.9177318242768687</v>
       </c>
       <c r="G109">
-        <v>-0.007000430162990123</v>
+        <v>-0.007000429909016503</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -3000,10 +2974,10 @@
         <v>0.893258559856304</v>
       </c>
       <c r="F110">
-        <v>0.9313781885500557</v>
+        <v>0.9313781892874846</v>
       </c>
       <c r="G110">
-        <v>-0.03811962869375174</v>
+        <v>-0.03811962943118063</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -3023,10 +2997,10 @@
         <v>0.907282539469667</v>
       </c>
       <c r="F111">
-        <v>0.9329378620346761</v>
+        <v>0.9329378624194509</v>
       </c>
       <c r="G111">
-        <v>-0.02565532256500913</v>
+        <v>-0.0256553229497839</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -3046,10 +3020,10 @@
         <v>0.9173024150657642</v>
       </c>
       <c r="F112">
-        <v>0.9353516079411455</v>
+        <v>0.935351607939704</v>
       </c>
       <c r="G112">
-        <v>-0.01804919287538131</v>
+        <v>-0.0180491928739398</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -3069,10 +3043,10 @@
         <v>0.9120195370430441</v>
       </c>
       <c r="F113">
-        <v>0.9282390799597262</v>
+        <v>0.9282390802809342</v>
       </c>
       <c r="G113">
-        <v>-0.01621954291668215</v>
+        <v>-0.0162195432378901</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -3089,13 +3063,13 @@
         <v>1990</v>
       </c>
       <c r="E114">
-        <v>10.44421893148241</v>
+        <v>10.55961036583401</v>
       </c>
       <c r="F114">
-        <v>12.13865402238989</v>
+        <v>13.81434111927517</v>
       </c>
       <c r="G114">
-        <v>-1.694435090907481</v>
+        <v>-3.254730753441164</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -3112,13 +3086,13 @@
         <v>1991</v>
       </c>
       <c r="E115">
-        <v>11.50966321945786</v>
+        <v>11.70209477787056</v>
       </c>
       <c r="F115">
-        <v>12.62985807263324</v>
+        <v>14.40166642947309</v>
       </c>
       <c r="G115">
-        <v>-1.120194853175381</v>
+        <v>-2.699571651602531</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -3135,13 +3109,13 @@
         <v>1992</v>
       </c>
       <c r="E116">
-        <v>12.92261038501988</v>
+        <v>13.1512353975563</v>
       </c>
       <c r="F116">
-        <v>13.55443353633743</v>
+        <v>16.03921527038666</v>
       </c>
       <c r="G116">
-        <v>-0.6318231513175547</v>
+        <v>-2.887979872830359</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -3158,13 +3132,13 @@
         <v>1993</v>
       </c>
       <c r="E117">
-        <v>13.08593023451205</v>
+        <v>13.38313279262732</v>
       </c>
       <c r="F117">
-        <v>13.83137917294557</v>
+        <v>16.64616371876692</v>
       </c>
       <c r="G117">
-        <v>-0.7454489384335155</v>
+        <v>-3.263030926139601</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -3181,13 +3155,13 @@
         <v>1994</v>
       </c>
       <c r="E118">
-        <v>14.05848672720817</v>
+        <v>14.38670679027616</v>
       </c>
       <c r="F118">
-        <v>14.40103093825329</v>
+        <v>18.0975481730718</v>
       </c>
       <c r="G118">
-        <v>-0.3425442110451176</v>
+        <v>-3.710841382795632</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -3204,13 +3178,13 @@
         <v>1995</v>
       </c>
       <c r="E119">
-        <v>14.65527652363886</v>
+        <v>14.73861807792662</v>
       </c>
       <c r="F119">
-        <v>15.33705379520099</v>
+        <v>20.0814025368609</v>
       </c>
       <c r="G119">
-        <v>-0.6817772715621278</v>
+        <v>-5.342784458934277</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -3227,13 +3201,13 @@
         <v>1996</v>
       </c>
       <c r="E120">
-        <v>14.58889291605732</v>
+        <v>14.78958698253564</v>
       </c>
       <c r="F120">
-        <v>16.25500363006422</v>
+        <v>21.99400518956544</v>
       </c>
       <c r="G120">
-        <v>-1.666110714006898</v>
+        <v>-7.2044182070298</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -3250,13 +3224,13 @@
         <v>1997</v>
       </c>
       <c r="E121">
-        <v>15.06521582034969</v>
+        <v>15.23827197367915</v>
       </c>
       <c r="F121">
-        <v>17.2477861386876</v>
+        <v>25.25917786513316</v>
       </c>
       <c r="G121">
-        <v>-2.182570318337914</v>
+        <v>-10.02090589145401</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -3273,13 +3247,13 @@
         <v>1998</v>
       </c>
       <c r="E122">
-        <v>15.18984433243649</v>
+        <v>15.37351057092645</v>
       </c>
       <c r="F122">
-        <v>17.33445450540114</v>
+        <v>25.72206541174786</v>
       </c>
       <c r="G122">
-        <v>-2.144610172964654</v>
+        <v>-10.34855484082141</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -3296,13 +3270,13 @@
         <v>1999</v>
       </c>
       <c r="E123">
-        <v>14.86240428386223</v>
+        <v>15.05988243142924</v>
       </c>
       <c r="F123">
-        <v>17.37104550384032</v>
+        <v>25.64390410805472</v>
       </c>
       <c r="G123">
-        <v>-2.508641219978085</v>
+        <v>-10.58402167662548</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -3319,13 +3293,13 @@
         <v>2000</v>
       </c>
       <c r="E124">
-        <v>16.20255782933533</v>
+        <v>16.5161566862657</v>
       </c>
       <c r="F124">
-        <v>18.6283280067431</v>
+        <v>29.7412607228633</v>
       </c>
       <c r="G124">
-        <v>-2.425770177407763</v>
+        <v>-13.2251040365976</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -3342,13 +3316,13 @@
         <v>2001</v>
       </c>
       <c r="E125">
-        <v>17.11381637007166</v>
+        <v>17.54709214511003</v>
       </c>
       <c r="F125">
-        <v>19.35893767324234</v>
+        <v>32.5791358897964</v>
       </c>
       <c r="G125">
-        <v>-2.245121303170684</v>
+        <v>-15.03204374468638</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -3365,13 +3339,13 @@
         <v>2002</v>
       </c>
       <c r="E126">
-        <v>17.43056964456489</v>
+        <v>17.74570214416709</v>
       </c>
       <c r="F126">
-        <v>19.63916697285452</v>
+        <v>34.93554885640838</v>
       </c>
       <c r="G126">
-        <v>-2.208597328289628</v>
+        <v>-17.18984671224129</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -3388,13 +3362,13 @@
         <v>2003</v>
       </c>
       <c r="E127">
-        <v>17.86912864503124</v>
+        <v>18.17119148840575</v>
       </c>
       <c r="F127">
-        <v>20.04636518904492</v>
+        <v>35.26848339712399</v>
       </c>
       <c r="G127">
-        <v>-2.177236544013684</v>
+        <v>-17.09729190871824</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -3411,13 +3385,13 @@
         <v>2004</v>
       </c>
       <c r="E128">
-        <v>18.66065286617572</v>
+        <v>18.87929938121229</v>
       </c>
       <c r="F128">
-        <v>20.93360682771728</v>
+        <v>40.24391820760753</v>
       </c>
       <c r="G128">
-        <v>-2.27295396154156</v>
+        <v>-21.36461882639524</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -3434,13 +3408,13 @@
         <v>2005</v>
       </c>
       <c r="E129">
-        <v>19.91285101425019</v>
+        <v>20.06115148016324</v>
       </c>
       <c r="F129">
-        <v>21.45926015600574</v>
+        <v>40.8300938212125</v>
       </c>
       <c r="G129">
-        <v>-1.546409141755554</v>
+        <v>-20.76894234104926</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -3457,13 +3431,13 @@
         <v>2006</v>
       </c>
       <c r="E130">
-        <v>20.94014539493338</v>
+        <v>21.23329510557974</v>
       </c>
       <c r="F130">
-        <v>21.84479150925906</v>
+        <v>41.27993511371484</v>
       </c>
       <c r="G130">
-        <v>-0.9046461143256757</v>
+        <v>-20.04664000813511</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -3480,13 +3454,13 @@
         <v>2007</v>
       </c>
       <c r="E131">
-        <v>20.61381007482522</v>
+        <v>20.90698398214961</v>
       </c>
       <c r="F131">
-        <v>22.24206302337927</v>
+        <v>42.42053843898897</v>
       </c>
       <c r="G131">
-        <v>-1.628252948554049</v>
+        <v>-21.51355445683936</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -3503,13 +3477,13 @@
         <v>2008</v>
       </c>
       <c r="E132">
-        <v>20.89371867083874</v>
+        <v>21.43241433696909</v>
       </c>
       <c r="F132">
-        <v>22.76458346495358</v>
+        <v>40.61341991614275</v>
       </c>
       <c r="G132">
-        <v>-1.870864794114837</v>
+        <v>-19.18100557917366</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -3526,13 +3500,13 @@
         <v>2009</v>
       </c>
       <c r="E133">
-        <v>20.82775039998421</v>
+        <v>21.45278578374574</v>
       </c>
       <c r="F133">
-        <v>21.99291333496449</v>
+        <v>36.42587734151411</v>
       </c>
       <c r="G133">
-        <v>-1.16516293498028</v>
+        <v>-14.97309155776837</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -3549,13 +3523,13 @@
         <v>2010</v>
       </c>
       <c r="E134">
-        <v>20.11024225561715</v>
+        <v>20.441937382259</v>
       </c>
       <c r="F134">
-        <v>22.39085644468673</v>
+        <v>31.5132610919008</v>
       </c>
       <c r="G134">
-        <v>-2.280614189069581</v>
+        <v>-11.0713237096418</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -3572,13 +3546,13 @@
         <v>2011</v>
       </c>
       <c r="E135">
-        <v>21.81115921851643</v>
+        <v>22.26155053018847</v>
       </c>
       <c r="F135">
-        <v>24.30738723787483</v>
+        <v>36.58558629870319</v>
       </c>
       <c r="G135">
-        <v>-2.496228019358401</v>
+        <v>-14.32403576851472</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -3595,13 +3569,13 @@
         <v>2012</v>
       </c>
       <c r="E136">
-        <v>22.22241659872683</v>
+        <v>22.57883648506208</v>
       </c>
       <c r="F136">
-        <v>24.09123066729878</v>
+        <v>32.24597557717168</v>
       </c>
       <c r="G136">
-        <v>-1.868814068571957</v>
+        <v>-9.667139092109604</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -3618,13 +3592,13 @@
         <v>2013</v>
       </c>
       <c r="E137">
-        <v>23.57540211823902</v>
+        <v>23.98578737917089</v>
       </c>
       <c r="F137">
-        <v>25.27869547708129</v>
+        <v>35.95211848780518</v>
       </c>
       <c r="G137">
-        <v>-1.70329335884227</v>
+        <v>-11.96633110863429</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -3641,13 +3615,13 @@
         <v>2014</v>
       </c>
       <c r="E138">
-        <v>25.68045141693354</v>
+        <v>25.98764900336978</v>
       </c>
       <c r="F138">
-        <v>27.49677190480819</v>
+        <v>44.54444152747186</v>
       </c>
       <c r="G138">
-        <v>-1.816320487874648</v>
+        <v>-18.55679252410208</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -3664,13 +3638,13 @@
         <v>2015</v>
       </c>
       <c r="E139">
-        <v>28.55496062193244</v>
+        <v>28.93519221352137</v>
       </c>
       <c r="F139">
-        <v>28.10584238249005</v>
+        <v>38.41675166459511</v>
       </c>
       <c r="G139">
-        <v>0.4491182394423952</v>
+        <v>-9.481559451073743</v>
       </c>
     </row>
   </sheetData>
@@ -3687,40 +3661,40 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3741,25 +3715,25 @@
         <v>2019</v>
       </c>
       <c r="F2">
-        <v>0.02530937959912019</v>
+        <v>0.02532784397665466</v>
       </c>
       <c r="G2">
-        <v>42.69611969685105</v>
+        <v>42.75998022855752</v>
       </c>
       <c r="H2">
-        <v>0.001466780711313291</v>
+        <v>0.001432113766272995</v>
       </c>
       <c r="I2">
-        <v>0.02806288907246639</v>
+        <v>0.0280575143787688</v>
       </c>
       <c r="J2">
-        <v>19.13230032002542</v>
+        <v>19.59167982288661</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>2.530937959912019</v>
+        <v>2.532784397665465</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -3779,25 +3753,25 @@
         <v>2019</v>
       </c>
       <c r="F3">
-        <v>-0.0213403315400211</v>
+        <v>-0.02134658235258359</v>
       </c>
       <c r="G3">
-        <v>-2.279378351400225</v>
+        <v>-2.280029539711471</v>
       </c>
       <c r="H3">
-        <v>0.003161949655122997</v>
+        <v>0.003160987500628101</v>
       </c>
       <c r="I3">
-        <v>0.02462279018676942</v>
+        <v>0.02462864330948595</v>
       </c>
       <c r="J3">
-        <v>7.787217657585259</v>
+        <v>7.791439638591464</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>-2.134033154002111</v>
+        <v>-2.134658235258359</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -3817,22 +3791,22 @@
         <v>2019</v>
       </c>
       <c r="F4">
-        <v>789.0116555312904</v>
+        <v>911.2263978881209</v>
       </c>
       <c r="G4">
-        <v>3.144642474119467</v>
+        <v>3.528376452965006</v>
       </c>
       <c r="H4">
-        <v>571.5170254546947</v>
+        <v>531.5104660290007</v>
       </c>
       <c r="I4">
-        <v>1099.881305189108</v>
+        <v>1129.340695396944</v>
       </c>
       <c r="J4">
-        <v>1.924494382847214</v>
+        <v>2.124776025267062</v>
       </c>
       <c r="K4">
-        <v>0.8</v>
+        <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -3852,25 +3826,25 @@
         <v>2015</v>
       </c>
       <c r="F5">
-        <v>0.01822269034906056</v>
+        <v>0.01822275601600201</v>
       </c>
       <c r="G5">
-        <v>25.48326767467013</v>
+        <v>25.48338780698378</v>
       </c>
       <c r="H5">
-        <v>0.01357743658995537</v>
+        <v>0.01357744019880436</v>
       </c>
       <c r="I5">
-        <v>0.02035393641916204</v>
+        <v>0.02035400544055883</v>
       </c>
       <c r="J5">
-        <v>1.4991000903823</v>
+        <v>1.499104775460636</v>
       </c>
       <c r="K5">
-        <v>0.1666666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="L5">
-        <v>1.822269034906056</v>
+        <v>1.822275601600201</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -3890,25 +3864,25 @@
         <v>2015</v>
       </c>
       <c r="F6">
-        <v>-0.02010666308700644</v>
+        <v>-0.02010666321071131</v>
       </c>
       <c r="G6">
-        <v>-2.160634615233468</v>
+        <v>-2.160634627764196</v>
       </c>
       <c r="H6">
-        <v>0.01425753112026511</v>
+        <v>0.01425753117904609</v>
       </c>
       <c r="I6">
-        <v>0.02233228423887432</v>
+        <v>0.02233228449587008</v>
       </c>
       <c r="J6">
-        <v>1.566350025856304</v>
+        <v>1.566350037423817</v>
       </c>
       <c r="K6">
         <v>0.3333333333333333</v>
       </c>
       <c r="L6">
-        <v>-2.010666308700644</v>
+        <v>-2.010666321071131</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -3928,19 +3902,19 @@
         <v>2015</v>
       </c>
       <c r="F7">
-        <v>-1.619358647379077</v>
+        <v>-12.51119694234604</v>
       </c>
       <c r="G7">
-        <v>-6.659635478271006</v>
+        <v>-33.98128150747707</v>
       </c>
       <c r="H7">
-        <v>1.739588953558521</v>
+        <v>13.75480976444275</v>
       </c>
       <c r="I7">
-        <v>1.88532742518186</v>
+        <v>12.90124920447528</v>
       </c>
       <c r="J7">
-        <v>1.083777533379488</v>
+        <v>0.9379445754187027</v>
       </c>
       <c r="K7">
         <v>0.4166666666666667</v>
@@ -3960,22 +3934,22 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3984,16 +3958,16 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>1.822269034906056</v>
+        <v>1.822275601600201</v>
       </c>
       <c r="C2">
-        <v>-2.010666308700644</v>
+        <v>-2.010666321071131</v>
       </c>
       <c r="D2">
-        <v>-1.619358647379077</v>
+        <v>-12.51119694234604</v>
       </c>
       <c r="E2">
-        <v>-6.659635478271006</v>
+        <v>-33.98128150747707</v>
       </c>
       <c r="F2" t="s">
         <v>28</v>
@@ -4004,16 +3978,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>2.530937959912019</v>
+        <v>2.532784397665465</v>
       </c>
       <c r="C3">
-        <v>-2.134033154002111</v>
+        <v>-2.134658235258359</v>
       </c>
       <c r="D3">
-        <v>789.0116555312904</v>
+        <v>911.2263978881209</v>
       </c>
       <c r="E3">
-        <v>3.144642474119467</v>
+        <v>3.528376452965006</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -4033,40 +4007,40 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -4087,25 +4061,25 @@
         <v>2019</v>
       </c>
       <c r="F2">
-        <v>0.007009587375176201</v>
+        <v>0.007297365409084998</v>
       </c>
       <c r="G2">
-        <v>4.035237298939539</v>
+        <v>4.206765147995309</v>
       </c>
       <c r="H2">
-        <v>0.009457024824047186</v>
+        <v>0.009471979747981408</v>
       </c>
       <c r="I2">
-        <v>0.009587276696935479</v>
+        <v>0.009811231397711862</v>
       </c>
       <c r="J2">
-        <v>1.013773028548798</v>
+        <v>1.035816340274878</v>
       </c>
       <c r="K2">
         <v>0.6666666666666666</v>
       </c>
       <c r="L2">
-        <v>0.7009587375176202</v>
+        <v>0.7297365409084998</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4125,25 +4099,25 @@
         <v>2019</v>
       </c>
       <c r="F3">
-        <v>-0.03989245536158898</v>
+        <v>-0.04234638544201628</v>
       </c>
       <c r="G3">
-        <v>-5.134202515526548</v>
+        <v>-5.433428597125665</v>
       </c>
       <c r="H3">
-        <v>0.009325287732901836</v>
+        <v>0.009673330136987351</v>
       </c>
       <c r="I3">
-        <v>0.04060412832389687</v>
+        <v>0.04301175021946676</v>
       </c>
       <c r="J3">
-        <v>4.354195761771064</v>
+        <v>4.44642637130777</v>
       </c>
       <c r="K3">
         <v>0.06666666666666667</v>
       </c>
       <c r="L3">
-        <v>-3.989245536158898</v>
+        <v>-4.234638544201628</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -4163,25 +4137,25 @@
         <v>2015</v>
       </c>
       <c r="F4">
-        <v>-0.04348639238995414</v>
+        <v>-0.04348492460497011</v>
       </c>
       <c r="G4">
-        <v>-9.916269975415672</v>
+        <v>-9.915960476081374</v>
       </c>
       <c r="H4">
-        <v>0.03105273545038395</v>
+        <v>0.03105285076416512</v>
       </c>
       <c r="I4">
-        <v>0.05083428229889892</v>
+        <v>0.05083295609916545</v>
       </c>
       <c r="J4">
-        <v>1.637030733737513</v>
+        <v>1.636981946849997</v>
       </c>
       <c r="K4">
         <v>0.4166666666666667</v>
       </c>
       <c r="L4">
-        <v>-4.348639238995414</v>
+        <v>-4.348492460497011</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -4201,25 +4175,25 @@
         <v>2015</v>
       </c>
       <c r="F5">
-        <v>0.05624371592406775</v>
+        <v>0.05624404142295391</v>
       </c>
       <c r="G5">
-        <v>12.02992614058695</v>
+        <v>12.03000383459898</v>
       </c>
       <c r="H5">
-        <v>0.02172778460574678</v>
+        <v>0.02172777454341443</v>
       </c>
       <c r="I5">
-        <v>0.0580892390959699</v>
+        <v>0.05808955536846841</v>
       </c>
       <c r="J5">
-        <v>2.673500319982272</v>
+        <v>2.67351611424351</v>
       </c>
       <c r="K5">
-        <v>0.1666666666666667</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="L5">
-        <v>5.624371592406774</v>
+        <v>5.624404142295391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>